<commit_message>
Integrate ExtentReports for reporting
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/EcommerceTestData.xlsx
+++ b/src/test/resources/testdata/EcommerceTestData.xlsx
@@ -9,25 +9,28 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8784"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8784" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="4" r:id="rId1"/>
     <sheet name="Register" sheetId="16" r:id="rId2"/>
-    <sheet name="CategoryAdd" sheetId="5" r:id="rId3"/>
-    <sheet name="CategoryEdit" sheetId="3" r:id="rId4"/>
-    <sheet name="CategoryDelete" sheetId="6" r:id="rId5"/>
-    <sheet name="ProductAdd" sheetId="2" r:id="rId6"/>
-    <sheet name="ProductEdit" sheetId="7" r:id="rId7"/>
-    <sheet name="ProductDelete" sheetId="1" r:id="rId8"/>
-    <sheet name="ChangeStatusOrder" sheetId="9" r:id="rId9"/>
-    <sheet name="BlogAdd" sheetId="8" r:id="rId10"/>
-    <sheet name="BlogEdit" sheetId="10" r:id="rId11"/>
-    <sheet name="BlogDelete" sheetId="11" r:id="rId12"/>
-    <sheet name="UserAdd" sheetId="12" r:id="rId13"/>
-    <sheet name="UserBlock" sheetId="13" r:id="rId14"/>
-    <sheet name="UserAsset" sheetId="14" r:id="rId15"/>
-    <sheet name="UserDelete" sheetId="15" r:id="rId16"/>
+    <sheet name="ChangeInfoUser" sheetId="17" r:id="rId3"/>
+    <sheet name="ChangePassword" sheetId="18" r:id="rId4"/>
+    <sheet name="CancelOrder" sheetId="19" r:id="rId5"/>
+    <sheet name="CategoryAdd" sheetId="5" r:id="rId6"/>
+    <sheet name="CategoryEdit" sheetId="3" r:id="rId7"/>
+    <sheet name="CategoryDelete" sheetId="6" r:id="rId8"/>
+    <sheet name="ProductAdd" sheetId="2" r:id="rId9"/>
+    <sheet name="ProductEdit" sheetId="7" r:id="rId10"/>
+    <sheet name="ProductDelete" sheetId="1" r:id="rId11"/>
+    <sheet name="ChangeStatusOrder" sheetId="9" r:id="rId12"/>
+    <sheet name="BlogAdd" sheetId="8" r:id="rId13"/>
+    <sheet name="BlogEdit" sheetId="10" r:id="rId14"/>
+    <sheet name="BlogDelete" sheetId="11" r:id="rId15"/>
+    <sheet name="UserAdd" sheetId="12" r:id="rId16"/>
+    <sheet name="UserBlock" sheetId="13" r:id="rId17"/>
+    <sheet name="UserAsset" sheetId="14" r:id="rId18"/>
+    <sheet name="UserDelete" sheetId="15" r:id="rId19"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -39,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="101">
   <si>
     <t>thanhhieu@gmail.com</t>
   </si>
@@ -230,15 +233,9 @@
     <t>status</t>
   </si>
   <si>
-    <t>#688766f4</t>
-  </si>
-  <si>
     <t>Đang giao</t>
   </si>
   <si>
-    <t>#688766f5</t>
-  </si>
-  <si>
     <t>title</t>
   </si>
   <si>
@@ -302,32 +299,59 @@
     <t>1234567LJ</t>
   </si>
   <si>
-    <t>testCaseId</t>
-  </si>
-  <si>
-    <t>TC01</t>
-  </si>
-  <si>
-    <t>TC02</t>
-  </si>
-  <si>
-    <t>TC03</t>
-  </si>
-  <si>
-    <t>TC04</t>
-  </si>
-  <si>
-    <t>TC05</t>
-  </si>
-  <si>
     <t>0914549857L</t>
+  </si>
+  <si>
+    <t>689073e2</t>
+  </si>
+  <si>
+    <t>689073e3</t>
+  </si>
+  <si>
+    <t>testname2</t>
+  </si>
+  <si>
+    <t>password_current</t>
+  </si>
+  <si>
+    <t>password_new</t>
+  </si>
+  <si>
+    <t>missing_password_current</t>
+  </si>
+  <si>
+    <t>missing_password_new</t>
+  </si>
+  <si>
+    <t>password_notcorrect</t>
+  </si>
+  <si>
+    <t>test2@gmail.com</t>
+  </si>
+  <si>
+    <t>test3@gmail.com</t>
+  </si>
+  <si>
+    <t>0914549857H</t>
+  </si>
+  <si>
+    <t>test5@gmail</t>
+  </si>
+  <si>
+    <t>0914549857</t>
+  </si>
+  <si>
+    <t>6890f3fdbe927af54c18f295</t>
+  </si>
+  <si>
+    <t>6890f3fdbe927af54c18f296</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -365,6 +389,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -393,7 +423,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -415,21 +445,18 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="11" fontId="3" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -711,69 +738,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.5546875" style="12" customWidth="1"/>
-    <col min="2" max="2" width="23.109375" customWidth="1"/>
-    <col min="3" max="3" width="22.6640625" customWidth="1"/>
-    <col min="4" max="4" width="17.21875" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" customWidth="1"/>
+    <col min="3" max="3" width="17.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
-        <v>87</v>
+    <row r="1" spans="1:3" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="B2" s="3" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
+      <c r="B2" s="2" t="s">
+        <v>85</v>
+      </c>
       <c r="C2" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="B3" s="2"/>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>85</v>
+      </c>
       <c r="C3" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D3" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="13"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="13"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="A2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -781,10 +792,375 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="6" width="13.77734375" customWidth="1"/>
+    <col min="7" max="8" width="12" customWidth="1"/>
+    <col min="9" max="10" width="41" customWidth="1"/>
+    <col min="11" max="11" width="20.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="2">
+        <v>50</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="2">
+        <v>40</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="2">
+        <v>30</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="2">
+        <v>30</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="2">
+        <v>30</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="28.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.77734375" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="A1:XFD1048576"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -797,10 +1173,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>8</v>
@@ -811,10 +1187,10 @@
     </row>
     <row r="2" spans="1:4" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>10</v>
@@ -826,37 +1202,37 @@
     <row r="3" spans="1:4" ht="60.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="64.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="64.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -864,7 +1240,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
@@ -882,16 +1258,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -899,16 +1275,16 @@
     </row>
     <row r="2" spans="1:5" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>4</v>
@@ -917,31 +1293,31 @@
     <row r="3" spans="1:5" ht="60.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="64.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="64.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -957,12 +1333,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -973,7 +1349,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>3</v>
@@ -981,7 +1357,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
@@ -989,7 +1365,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>13</v>
@@ -1007,12 +1383,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="A1:XFD1048576"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1042,10 +1418,10 @@
         <v>9</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>4</v>
@@ -1054,10 +1430,10 @@
     <row r="3" spans="1:4" ht="60.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>12</v>
@@ -1069,7 +1445,7 @@
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>5</v>
@@ -1080,13 +1456,13 @@
         <v>41</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="64.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -1094,11 +1470,11 @@
         <v>49</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1110,7 +1486,93 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.109375" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="60.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.109375" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="60.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -1141,89 +1603,9 @@
       </c>
     </row>
     <row r="3" spans="1:2" ht="60.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="18.109375" customWidth="1"/>
-    <col min="2" max="2" width="17" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="54" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="60.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="18.109375" customWidth="1"/>
-    <col min="2" max="2" width="17" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="54" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="60.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
+      <c r="A3" s="2" t="s">
+        <v>88</v>
+      </c>
       <c r="B3" s="2" t="s">
         <v>13</v>
       </c>
@@ -1235,121 +1617,102 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.5546875" style="12" customWidth="1"/>
-    <col min="2" max="2" width="18.109375" customWidth="1"/>
-    <col min="3" max="3" width="27.77734375" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" customWidth="1"/>
-    <col min="5" max="5" width="17" customWidth="1"/>
+    <col min="1" max="1" width="18.109375" customWidth="1"/>
+    <col min="2" max="2" width="27.77734375" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
-        <v>87</v>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="54" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="B2" s="2" t="s">
+    <row r="2" spans="1:4" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="60.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2"/>
+      <c r="B3" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="64.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="64.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="64.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="60.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="64.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="64.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="64.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2" t="s">
-        <v>81</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C5" r:id="rId2"/>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B5" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -1358,10 +1721,238 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="22.109375" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="12"/>
+      <c r="C4" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C6" s="2"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.21875" customWidth="1"/>
+    <col min="2" max="2" width="17.21875" customWidth="1"/>
+    <col min="3" max="3" width="23.21875" customWidth="1"/>
+    <col min="4" max="4" width="27.21875" customWidth="1"/>
+    <col min="5" max="5" width="22.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="D3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="D5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E6" s="2"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="27" customWidth="1"/>
+    <col min="2" max="2" width="21.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1443,7 +2034,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
@@ -1535,12 +2126,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B3" sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1585,12 +2176,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J10" sqref="A1:J10"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1852,369 +2443,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="6" width="13.77734375" customWidth="1"/>
-    <col min="7" max="8" width="12" customWidth="1"/>
-    <col min="9" max="10" width="41" customWidth="1"/>
-    <col min="11" max="11" width="20.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" s="2">
-        <v>50</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" s="2">
-        <v>40</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="2">
-        <v>0</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" s="2">
-        <v>30</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5" s="2">
-        <v>0</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D6" s="2">
-        <v>30</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" s="2">
-        <v>30</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="18.33203125" customWidth="1"/>
-    <col min="2" max="2" width="28.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B3" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="13.77734375" customWidth="1"/>
-    <col min="2" max="2" width="15.44140625" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>